<commit_message>
feat: adds task for case search input validation and performing search +entering form
</commit_message>
<xml_diff>
--- a/LocustScripts/client-cases-import-example.xlsx
+++ b/LocustScripts/client-cases-import-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathantang/dimagi-qa/LocustScripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B58211-CC87-F549-B9F8-CB1ACC67FEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E81FD0-141B-F14F-AA4E-2AF2B99BB6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52160" yWindow="11860" windowWidth="27640" windowHeight="15880" xr2:uid="{22C04250-D185-C84F-9606-9988992ED307}"/>
+    <workbookView xWindow="2100" yWindow="6500" windowWidth="27640" windowHeight="15880" xr2:uid="{22C04250-D185-C84F-9606-9988992ED307}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948E651E-69B2-1247-9EB6-6865D0935D9C}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,9 +548,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F3" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>